<commit_message>
df of v-a for the course, simplifying shit is not working
</commit_message>
<xml_diff>
--- a/Pre Research Works/Verbs-Assesmmnets.xlsx
+++ b/Pre Research Works/Verbs-Assesmmnets.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C186"/>
+  <dimension ref="A1:C181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,12 +451,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -481,12 +481,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>used</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -496,12 +496,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>think</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
         </is>
       </c>
     </row>
@@ -511,12 +511,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>surrounding</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -526,12 +526,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>according</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -541,12 +541,12 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>specified</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -556,12 +556,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>used</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -571,12 +571,12 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>think</t>
+          <t>gain</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
+          <t>['Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -586,12 +586,12 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>surrounding</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -601,12 +601,12 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>according</t>
+          <t>verify</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
         </is>
       </c>
     </row>
@@ -616,12 +616,12 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>specified</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -631,12 +631,12 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>programming</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -646,12 +646,12 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>gain</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>['Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -661,12 +661,12 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>programming</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -676,12 +676,12 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>verify</t>
+          <t>examine</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>visualize</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -706,12 +706,12 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>programming</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -721,12 +721,12 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -736,12 +736,12 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>programming</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -751,12 +751,12 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>examine</t>
+          <t>programming</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -766,12 +766,12 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>visualize</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -781,12 +781,12 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>given</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -811,12 +811,12 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -826,12 +826,12 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>programming</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -841,12 +841,12 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>given</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -856,12 +856,12 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>given</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -871,12 +871,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -886,12 +886,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>infer</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -901,12 +901,12 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>analyze</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -916,12 +916,12 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>given</t>
+          <t>designing</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -931,12 +931,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>including</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
         </is>
       </c>
     </row>
@@ -946,12 +946,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -961,12 +961,12 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>infer</t>
+          <t>deciding</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
         </is>
       </c>
     </row>
@@ -976,12 +976,12 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>analyze</t>
+          <t>know</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
         </is>
       </c>
     </row>
@@ -991,12 +991,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>designing</t>
+          <t>do</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1006,12 +1006,12 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>including</t>
+          <t>admit</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1021,12 +1021,12 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>understanding</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1036,12 +1036,12 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>deciding</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1051,12 +1051,12 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>know</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1066,12 +1066,12 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>do</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1081,12 +1081,12 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>admit</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1096,12 +1096,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>understanding</t>
+          <t>sampling</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1111,12 +1111,12 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>develop</t>
+          <t>testing</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1126,12 +1126,12 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>estimate</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1141,12 +1141,12 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1156,12 +1156,12 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1171,12 +1171,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>sampling</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1186,12 +1186,12 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>testing</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1201,7 +1201,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>estimate</t>
+          <t>create</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -1216,12 +1216,12 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>describethemaintechnologiesandmethodscurrentlyusedincreating</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1231,12 +1231,12 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>inherent</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1261,12 +1261,12 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1276,12 +1276,12 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>create</t>
+          <t>writing</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
         </is>
       </c>
     </row>
@@ -1291,12 +1291,12 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>describethemaintechnologiesandmethodscurrentlyusedincreating</t>
+          <t>programming</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>inherent</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
@@ -1321,12 +1321,12 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1336,12 +1336,12 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>develop</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1351,12 +1351,12 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>writing</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1366,12 +1366,12 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>programming</t>
+          <t>are</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1381,12 +1381,12 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>formulated</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1396,12 +1396,12 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>develop</t>
+          <t>solved</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1411,12 +1411,12 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1426,12 +1426,12 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1441,12 +1441,12 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>are</t>
+          <t>formulate</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1456,12 +1456,12 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>formulated</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1471,12 +1471,12 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>solved</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>use</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
@@ -1516,12 +1516,12 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>formulate</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1531,12 +1531,12 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>describe</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
@@ -1576,12 +1576,12 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>use</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1591,12 +1591,12 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>classified</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>describe</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
@@ -1621,12 +1621,12 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>computing</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1636,12 +1636,12 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1651,12 +1651,12 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1666,12 +1666,12 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>classified</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1681,12 +1681,12 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>present</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1696,12 +1696,12 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>computing</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1711,7 +1711,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>analyse</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -1726,12 +1726,12 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>differentiate</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1741,12 +1741,12 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>forecast</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1756,12 +1756,12 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>present</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1771,12 +1771,12 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>(ann)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1786,12 +1786,12 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>analyse</t>
+          <t>implementing</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1801,12 +1801,12 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>differentiate</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1816,12 +1816,12 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>forecast</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1831,12 +1831,12 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>(ann)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>(ann)</t>
+          <t>thei</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -1861,12 +1861,12 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>implementing</t>
+          <t>(cnn)</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1876,12 +1876,12 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>evaluatethechallengesintraining</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1891,12 +1891,12 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>(rnn)</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1906,12 +1906,12 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>(ann)</t>
+          <t>create</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1921,12 +1921,12 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>thei</t>
+          <t>analysis.</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1936,12 +1936,12 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>(cnn)</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1951,12 +1951,12 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>evaluatethechallengesintraining</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1966,12 +1966,12 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>(rnn)</t>
+          <t>reporting</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
         </is>
       </c>
     </row>
@@ -1981,12 +1981,12 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>create</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -1996,12 +1996,12 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>analysis.</t>
+          <t>associated</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2011,12 +2011,12 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>illustrate</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
@@ -2041,12 +2041,12 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>reporting</t>
+          <t>constructing</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2056,12 +2056,12 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>linking</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2071,12 +2071,12 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>associated</t>
+          <t>utilizing</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2086,7 +2086,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>illustrate</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
@@ -2101,12 +2101,12 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>illustrate</t>
+          <t>constructing</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2116,12 +2116,12 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>constructing</t>
+          <t>linking</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2131,12 +2131,12 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>linking</t>
+          <t>utilizing</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2146,12 +2146,12 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>utilizing</t>
+          <t>describe</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2161,12 +2161,12 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>illustrate</t>
+          <t>computing</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2176,7 +2176,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>constructing</t>
+          <t>processing</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -2191,12 +2191,12 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>linking</t>
+          <t>analyze</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2206,12 +2206,12 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>utilizing</t>
+          <t>based</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
         </is>
       </c>
     </row>
@@ -2221,12 +2221,12 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>describe</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2236,12 +2236,12 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>computing</t>
+          <t>be</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>processing</t>
+          <t>implementing</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
@@ -2266,12 +2266,12 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>analyze</t>
+          <t>applying</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2281,12 +2281,12 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>based</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2296,12 +2296,12 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>knowledgeof</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2311,12 +2311,12 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>be</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2326,12 +2326,12 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>implementing</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>applying</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -2356,12 +2356,12 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>developing</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2371,12 +2371,12 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>knowledgeof</t>
+          <t>integrating</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2386,12 +2386,12 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>perform</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2401,12 +2401,12 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>advanced</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2416,12 +2416,12 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2431,12 +2431,12 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>developing</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2446,12 +2446,12 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>integrating</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2461,12 +2461,12 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>perform</t>
+          <t>use</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2476,12 +2476,12 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>advanced</t>
+          <t>processing</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2491,12 +2491,12 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2506,12 +2506,12 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>interpret</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -2536,12 +2536,12 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>use</t>
+          <t>adequacy</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
         </is>
       </c>
     </row>
@@ -2551,12 +2551,12 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>processing</t>
+          <t>model.</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -2581,12 +2581,12 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>distributed</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2596,7 +2596,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>interpret</t>
+          <t>demonstrate</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -2611,12 +2611,12 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>adequacy</t>
+          <t>involved</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>['Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2626,12 +2626,12 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>model.</t>
+          <t>identify</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2641,12 +2641,12 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>be</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2656,12 +2656,12 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>distributed</t>
+          <t>organized</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -2671,12 +2671,12 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>demonstrate</t>
+          <t>displayed.</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -2686,12 +2686,12 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>involved</t>
+          <t>interpret</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2701,12 +2701,12 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>identify</t>
+          <t>based</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
         </is>
       </c>
     </row>
@@ -2716,12 +2716,12 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>be</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2731,12 +2731,12 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>organized</t>
+          <t>computing</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2746,12 +2746,12 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>displayed.</t>
+          <t>classify</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>['Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
         </is>
       </c>
     </row>
@@ -2761,12 +2761,12 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>interpret</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2776,12 +2776,12 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>based</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>['Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2791,12 +2791,12 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2806,12 +2806,12 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>computing</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2821,12 +2821,12 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>classify</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -2851,12 +2851,12 @@
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>evaluate</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2881,12 +2881,12 @@
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>grasp</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2896,12 +2896,12 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>solve</t>
+          <t>including</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
         </is>
       </c>
     </row>
@@ -2911,12 +2911,12 @@
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2926,7 +2926,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>evaluate</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
@@ -2956,12 +2956,12 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>grasp</t>
+          <t>represent</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2971,12 +2971,12 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>including</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>['Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -2986,12 +2986,12 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>apply</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3001,7 +3001,7 @@
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>develop</t>
+          <t>evaluate</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
@@ -3016,12 +3016,12 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>generated</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3031,12 +3031,12 @@
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>represent</t>
+          <t>using</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>learning</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -3061,12 +3061,12 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>understand</t>
+          <t>solving</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3076,12 +3076,12 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>evaluate</t>
+          <t>understand</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3091,12 +3091,12 @@
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>generated</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3106,12 +3106,12 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>using</t>
+          <t>develop</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3121,12 +3121,12 @@
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>learning</t>
+          <t>apply</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
+          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>
       </c>
     </row>
@@ -3136,85 +3136,10 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>solving</t>
+          <t>solve</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
-        <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
-        </is>
-      </c>
-    </row>
-    <row r="182">
-      <c r="A182" s="1" t="n">
-        <v>180</v>
-      </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>understand</t>
-        </is>
-      </c>
-      <c r="C182" t="inlineStr">
-        <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as papers, exams, problem sets, class discussions, or concept maps that require students to: summarize readings, films, or speeches • compare and contrast two or more theories, events, or processes • classify or categorize cases, elements, or events using established criteria • paraphrase documents or speeches • find or identify examples or illustrations of a concept or principle •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
-        </is>
-      </c>
-    </row>
-    <row r="183">
-      <c r="A183" s="1" t="n">
-        <v>181</v>
-      </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>develop</t>
-        </is>
-      </c>
-      <c r="C183" t="inlineStr">
-        <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
-        </is>
-      </c>
-    </row>
-    <row r="184">
-      <c r="A184" s="1" t="n">
-        <v>182</v>
-      </c>
-      <c r="B184" t="inlineStr">
-        <is>
-          <t>develop</t>
-        </is>
-      </c>
-      <c r="C184" t="inlineStr">
-        <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
-        </is>
-      </c>
-    </row>
-    <row r="185">
-      <c r="A185" s="1" t="n">
-        <v>183</v>
-      </c>
-      <c r="B185" t="inlineStr">
-        <is>
-          <t>apply</t>
-        </is>
-      </c>
-      <c r="C185" t="inlineStr">
-        <is>
-          <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as problem sets, performances, labs, prototyping, or simulations that require students to: use procedures to solve or complete familiar or unfamiliar tasks • determine which procedure(s) are most appropriate for a given task •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as journals, diaries, critiques, problem sets, product reviews, or studies that require students to: test, monitor, judge, or critique readings, performances, or products against established • criteria or standards', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
-        </is>
-      </c>
-    </row>
-    <row r="186">
-      <c r="A186" s="1" t="n">
-        <v>184</v>
-      </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>solve</t>
-        </is>
-      </c>
-      <c r="C186" t="inlineStr">
         <is>
           <t>['Objective test items such as fill-in-the-blank, matching, labeling, or multiple-choice questions that require students to: recall or recognize terms, facts, and concepts •', 'Activities such as case studies, critiques, labs, papers, projects, debates, or concept maps that require students to: discriminate or select relevant and irrelevant parts • determine how elements function together • determine bias, values, or underlying intent in presented material •', 'Activities such as research projects, musical compositions, performances, essays, business plans, website designs, or set designs that require students to: make, build, design or generate something new •']</t>
         </is>

</xml_diff>